<commit_message>
annex a examples added
</commit_message>
<xml_diff>
--- a/data/Penparcau_Butterfly.xlsx
+++ b/data/Penparcau_Butterfly.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13760" yWindow="2280" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="180" yWindow="460" windowWidth="21980" windowHeight="14140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -8408,7 +8408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL592"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="W487" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8442,7 +8442,7 @@
     <col min="28" max="28" width="36.1640625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="28.83203125" customWidth="1"/>
     <col min="32" max="32" width="46.83203125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="32.1640625" bestFit="1" customWidth="1"/>

</xml_diff>